<commit_message>
Update 1 file TaskofProject-Calculator
</commit_message>
<xml_diff>
--- a/TaskofProjectDemo-Calculator.xlsx
+++ b/TaskofProjectDemo-Calculator.xlsx
@@ -37,22 +37,22 @@
     <t>#Layout</t>
   </si>
   <si>
-    <t>   - LinearLayout</t>
-  </si>
-  <si>
-    <t>   - TextView</t>
-  </si>
-  <si>
-    <t>   - Button</t>
+    <t>- LinearLayout</t>
+  </si>
+  <si>
+    <t>- TextView</t>
+  </si>
+  <si>
+    <t>- Button</t>
   </si>
   <si>
     <t>#Calculator</t>
   </si>
   <si>
-    <t>   - Activity</t>
-  </si>
-  <si>
-    <t>   - Ký pháp Balan - biểu thức tiền tố, hậu tố</t>
+    <t>- Activity</t>
+  </si>
+  <si>
+    <t>- Ký pháp Balan - biểu thức tiền tố, hậu tố</t>
   </si>
   <si>
     <t>#Tìm hiểu ký pháp Balan</t>
@@ -67,7 +67,7 @@
     <t>#Tìm hiểu SQLite</t>
   </si>
   <si>
-    <t>   - ListView</t>
+    <t>- ListView</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -185,6 +185,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +280,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -317,66 +321,66 @@
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="n">
@@ -385,42 +389,42 @@
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>